<commit_message>
added details to doc and edited excel
</commit_message>
<xml_diff>
--- a/4_ProjectManagement/Studies/FP_study_Erica.xlsx
+++ b/4_ProjectManagement/Studies/FP_study_Erica.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.tinti\Documents\personali\università\SE2\SE2project\4_ProjectManagement\Studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Documents\2016_SE2_project\SE2project\4_ProjectManagement\Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="UFP MODIF" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -278,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -301,25 +301,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -615,13 +618,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -1237,28 +1240,30 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.140625" style="1" customWidth="1"/>
-    <col min="2" max="6" width="9.140625" style="5"/>
+    <col min="2" max="2" width="14.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12" style="5" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="5"/>
     <col min="9" max="9" width="47.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -1344,8 +1349,8 @@
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="4">
         <v>2</v>
       </c>
@@ -1367,8 +1372,8 @@
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="5" t="s">
         <v>43</v>
       </c>
@@ -1377,8 +1382,8 @@
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
         <v>1</v>
@@ -1401,9 +1406,9 @@
         <v>36</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1412,25 +1417,25 @@
         <v>37</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="4">
         <v>2</v>
       </c>
@@ -1448,8 +1453,8 @@
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="5" t="s">
         <v>42</v>
       </c>
@@ -1459,11 +1464,11 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="5" t="s">
         <v>43</v>
       </c>
@@ -1476,8 +1481,8 @@
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4">
@@ -1499,8 +1504,8 @@
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
       <c r="F16" s="5" t="s">
         <v>42</v>
       </c>
@@ -1509,8 +1514,8 @@
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4">
@@ -1532,8 +1537,8 @@
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
       <c r="F18" s="5" t="s">
         <v>42</v>
       </c>
@@ -1542,8 +1547,8 @@
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="4">
         <v>2</v>
       </c>
@@ -1562,8 +1567,8 @@
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="5" t="s">
         <v>42</v>
       </c>
@@ -1572,8 +1577,8 @@
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="5" t="s">
         <v>42</v>
       </c>
@@ -1582,8 +1587,8 @@
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1596,8 +1601,8 @@
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
       <c r="F23" s="5" t="s">
         <v>42</v>
       </c>
@@ -1613,8 +1618,8 @@
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
       <c r="F24" s="5" t="s">
         <v>43</v>
       </c>
@@ -1627,8 +1632,8 @@
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="4">
         <v>2</v>
       </c>
@@ -1647,8 +1652,8 @@
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="5" t="s">
         <v>42</v>
       </c>
@@ -1657,14 +1662,14 @@
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H28" s="13">
+      <c r="H28" s="10">
         <f>SUM(H6:H25)</f>
         <v>47</v>
       </c>
@@ -1735,7 +1740,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H35" s="13">
+      <c r="H35" s="10">
         <f>SUM(H30:H34)</f>
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
added descriptions to FP
</commit_message>
<xml_diff>
--- a/4_ProjectManagement/Studies/FP_study_Erica.xlsx
+++ b/4_ProjectManagement/Studies/FP_study_Erica.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Documents\2016_SE2_project\SE2project\4_ProjectManagement\Studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.tinti\Documents\personali\università\SE2\SE2project\4_ProjectManagement\Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="UFP MODIF" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="72">
   <si>
     <t>[G8] The user should be able to access profile and payment method and make changes:</t>
   </si>
@@ -209,6 +209,39 @@
   </si>
   <si>
     <t>operator</t>
+  </si>
+  <si>
+    <t>The modification</t>
+  </si>
+  <si>
+    <t>view profile infos</t>
+  </si>
+  <si>
+    <t>modify profile infos</t>
+  </si>
+  <si>
+    <t>modify credit card infos</t>
+  </si>
+  <si>
+    <t>This is a simple operation. It involves many fields but only some query are needed. We assigned a weight of 3.</t>
+  </si>
+  <si>
+    <t>This function need to interact with the db and involves many fields. We assign it an average weight of 4.</t>
+  </si>
+  <si>
+    <t>This function need to interact with the db for saving info and  also with the bank to the credit card verify process. We assign it an average weight of 4.</t>
+  </si>
+  <si>
+    <t>to copy</t>
+  </si>
+  <si>
+    <t>This operation involves many components and many interactions with the db and several calculation. Then we consider it as a complex operation and we assign it a weight of 7.</t>
+  </si>
+  <si>
+    <t>It is a simple operation that involves a few fields, then we assign it a weight of 3,</t>
+  </si>
+  <si>
+    <t>This operation involves many components and requires several calculation. Then we consider it as an average complexity operation and we assign it a weight of 7.</t>
   </si>
 </sst>
 </file>
@@ -284,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -320,18 +353,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -627,13 +664,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -1246,13 +1283,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A30:A34"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,16 +1302,16 @@
     <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>23</v>
       </c>
@@ -1291,7 +1328,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
@@ -1311,7 +1348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
@@ -1331,7 +1368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>44</v>
       </c>
@@ -1353,8 +1390,11 @@
       <c r="H5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J5" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1364,164 +1404,186 @@
         <v>2</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6">
-        <f>D4</f>
-        <v>4</v>
+      <c r="F6" s="4">
+        <v>1</v>
       </c>
       <c r="H6">
-        <f>G6*D6</f>
-        <v>8</v>
+        <f>G7+G8+G9</f>
+        <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>35</v>
+      <c r="J6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="G7">
+        <f>D4</f>
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8">
+        <f>D4</f>
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9">
+        <f>D3</f>
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
         <v>1</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8">
+      <c r="F10" s="4"/>
+      <c r="G10">
         <f>E5</f>
         <v>7</v>
       </c>
-      <c r="H8">
-        <f>G8*E8</f>
+      <c r="H10">
+        <f>G10*E10</f>
         <v>7</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="4">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="4">
         <v>2</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="H12">
-        <f>G13*1+G14*1</f>
-        <v>7</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="H14">
+        <f>G15*1+G16*1</f>
+        <v>8</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15">
         <f>D3</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="J15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14">
-        <f>D4</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <f>F3</f>
-        <v>3</v>
-      </c>
-      <c r="H15">
-        <f>G15*F15</f>
-        <v>3</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>38</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
-      <c r="F16" s="5" t="s">
-        <v>42</v>
+      <c r="E16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16">
+        <f>E4</f>
+        <v>5</v>
+      </c>
+      <c r="J16" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1543,8 +1605,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>37</v>
+      <c r="A18" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1554,191 +1616,200 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="4">
-        <v>2</v>
-      </c>
+      <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
       <c r="G19">
         <f>F3</f>
         <v>3</v>
       </c>
       <c r="H19">
-        <f>G19*D19</f>
-        <v>6</v>
+        <f>G19*F19</f>
+        <v>3</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>39</v>
+      <c r="A20" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21">
+        <f>F3</f>
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <f>G21*D21</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="H22">
-        <f>G23*1+G24*1</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>53</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="F23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23">
+      <c r="D23" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="H24">
+        <f>G25*1+G26*1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="F25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25">
         <f>F3</f>
         <v>3</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="F24" s="5" t="s">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="F26" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G24">
+      <c r="G26">
         <f>F4</f>
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="4">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="4">
         <v>2</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27">
         <f>D3</f>
         <v>3</v>
       </c>
-      <c r="H25">
-        <f>G25*D25</f>
+      <c r="H27">
+        <f>G27*D27</f>
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H28" s="10">
-        <f>SUM(H6:H25)</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="10">
+        <f>SUM(H6:H27)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H30">
+      <c r="H32">
         <f>B4</f>
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H31">
+      <c r="H33">
         <f>B4</f>
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H32">
-        <f>B3</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H33">
-        <f>B3</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>60</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>42</v>
@@ -1749,17 +1820,41 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H35" s="10">
-        <f>SUM(H30:H34)</f>
+      <c r="A35" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35">
+        <f>B3</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36">
+        <f>B3</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="10">
+        <f>SUM(H32:H36)</f>
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added description to doc
</commit_message>
<xml_diff>
--- a/4_ProjectManagement/Studies/FP_study_Erica.xlsx
+++ b/4_ProjectManagement/Studies/FP_study_Erica.xlsx
@@ -384,6 +384,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,7 +394,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,13 +692,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -1314,10 +1314,10 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="J25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J37" sqref="J37"/>
+      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,13 +1331,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -1528,10 +1528,10 @@
       <c r="A11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17" t="s">
+      <c r="D11" s="18"/>
+      <c r="E11" s="18" t="s">
         <v>44</v>
       </c>
       <c r="J11" t="s">
@@ -1542,19 +1542,19 @@
       <c r="A12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1888,7 +1888,7 @@
         <f>B3</f>
         <v>7</v>
       </c>
-      <c r="J35" s="18" t="s">
+      <c r="J35" s="15" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>